<commit_message>
Added new reports - Trial Balance (With and Without balanced entries)
</commit_message>
<xml_diff>
--- a/trunk/application/PHPExcel-ADODB/reports/generated/TrialBalance.xlsx
+++ b/trunk/application/PHPExcel-ADODB/reports/generated/TrialBalance.xlsx
@@ -23,7 +23,7 @@
     <t>Trial Balance</t>
   </si>
   <si>
-    <t>As of February, 2010</t>
+    <t>As of February 24, 2010</t>
   </si>
   <si>
     <t>Debit</t>
@@ -328,7 +328,7 @@
       <color rgb="FF000000"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none">
         <fgColor rgb="FFFFFFFF"/>
@@ -347,6 +347,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -354,14 +360,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -371,6 +386,44 @@
   <dxfs count="0"/>
   <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3238500" cy="1905000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Example Chart" descr="Example Chart"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -664,7 +717,7 @@
   <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true">
-      <selection activeCell="B95" sqref="B95"/>
+      <selection activeCell="B96" sqref="B96:D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -673,31 +726,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="B6" s="1" t="s"/>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="2" t="s"/>
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -706,10 +759,10 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>1500</v>
+        <v>1400</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -999,20 +1052,20 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="4">
         <f>SUM(C8:C34)</f>
-        <v>1500</v>
-      </c>
-      <c r="D35">
+        <v>1400</v>
+      </c>
+      <c r="D35" s="4">
         <f>SUM(D8:D34)</f>
-        <v>650</v>
+        <v>550</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1021,10 +1074,10 @@
         <v>35</v>
       </c>
       <c r="C37">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>950</v>
+        <v>870</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1171,20 +1224,20 @@
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="4">
         <f>SUM(C37:C50)</f>
-        <v>80</v>
-      </c>
-      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="D51" s="4">
         <f>SUM(D37:D50)</f>
-        <v>950</v>
+        <v>870</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1222,20 +1275,20 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="4">
         <f>SUM(C53:C55)</f>
         <v>0</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="4">
         <f>SUM(D53:D55)</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1306,20 +1359,20 @@
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="4">
         <f>SUM(C58:C63)</f>
         <v>0</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="4">
         <f>SUM(D58:D63)</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1643,33 +1696,38 @@
       </c>
     </row>
     <row r="95" spans="1:4">
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="4">
         <f>SUM(C66:C94)</f>
         <v>20</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="4">
         <f>SUM(D66:D94)</f>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:4">
-      <c r="B96" t="s">
+      <c r="B96" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="2">
         <f>C35+C51+C56+C64+C95</f>
-        <v>1600</v>
-      </c>
-      <c r="D96">
+        <v>1420</v>
+      </c>
+      <c r="D96" s="2">
         <f>D35+D51+D56+D64+D95</f>
-        <v>1600</v>
+        <v>1420</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
@@ -1681,5 +1739,8 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="45" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
</xml_diff>